<commit_message>
Fixing UV Mapping Errors
</commit_message>
<xml_diff>
--- a/DevonThurgood_Drone_Timetable.xlsx
+++ b/DevonThurgood_Drone_Timetable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa7f6f3a4ff12958/Documents/Downloads/DGM-1660-Fall-2020-Devon-Thurgood/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{5037DE3C-66CE-4D02-AD33-613F11C43316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{183EE638-3AA1-433F-A839-AFBD9E8448C7}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{5037DE3C-66CE-4D02-AD33-613F11C43316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{88AB8E2C-9873-46CC-B617-FB2C790EC204}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
     <t>3 hours 45 minutes</t>
   </si>
   <si>
-    <t>1 hour 50 minutes</t>
+    <t>2 hour 55 minutes</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:Z64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="D38" sqref="D38:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>